<commit_message>
Performed 500MB transfer test (local)
</commit_message>
<xml_diff>
--- a/writeup/speed_test_transfer_local.xlsx
+++ b/writeup/speed_test_transfer_local.xlsx
@@ -136,7 +136,68 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Transfer</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Speeds for 100 MB Database</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -245,11 +306,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="784342416"/>
-        <c:axId val="784341872"/>
+        <c:axId val="-1813746208"/>
+        <c:axId val="-1813735328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="784342416"/>
+        <c:axId val="-1813746208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -348,12 +409,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="784341872"/>
+        <c:crossAx val="-1813735328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="784341872"/>
+        <c:axId val="-1813735328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -466,7 +527,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="784342416"/>
+        <c:crossAx val="-1813746208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1077,13 +1138,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>942975</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>536575</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -57425,11 +57486,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H17"/>
+  <dimension ref="B2:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -57661,20 +57720,32 @@
         <v>9.3087900000000001</v>
       </c>
       <c r="H10" s="3">
-        <f t="shared" ref="H10:H15" si="2">IFERROR(C10/G10,"")</f>
+        <f t="shared" ref="H10:H16" si="2">IFERROR(C10/G10,"")</f>
         <v>10.735397403959054</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1" t="str">
+      <c r="B11" s="1">
+        <v>75</v>
+      </c>
+      <c r="C11" s="4">
+        <v>499.54289999999997</v>
+      </c>
+      <c r="D11" s="1">
+        <v>500</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1023</v>
+      </c>
+      <c r="F11" s="1">
+        <v>23</v>
+      </c>
+      <c r="G11" s="3">
+        <v>66.025000000000006</v>
+      </c>
+      <c r="H11" s="3">
         <f t="shared" si="2"/>
-        <v/>
+        <v>7.5659659219992417</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.35">
@@ -57732,7 +57803,10 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="H16" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
@@ -57743,6 +57817,15 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
   </sheetData>
   <sortState ref="B3:H9">
     <sortCondition ref="D3:D9"/>

</xml_diff>